<commit_message>
Add CDC HIV template
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D8268D-7D5F-4445-8638-9B4851C7194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0792F0-DAAF-41AE-9CDE-0C62BF35E263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-3600" windowWidth="16440" windowHeight="29040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="824">
   <si>
     <t>sti</t>
   </si>
@@ -2779,6 +2779,12 @@
   </si>
   <si>
     <t>nmirasol@usbiotek.com</t>
+  </si>
+  <si>
+    <t>GONO, CHLA, HEPB, HEPC</t>
+  </si>
+  <si>
+    <t>GA_HIV_CDC.pdf</t>
   </si>
 </sst>
 </file>
@@ -4743,15 +4749,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0120148-02B5-41A0-B534-E70620D50CDF}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4780,13 +4788,38 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>822</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>821</v>
       </c>
       <c r="E2" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>820</v>
+      </c>
+      <c r="C3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" t="s">
+        <v>823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test destinations for MN and WI
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA580B55-37E0-45F0-8969-80D39D2C197E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461F6F07-CA8C-4502-BF81-01E8FC54FAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3555" windowWidth="15300" windowHeight="10020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="3" r:id="rId1"/>
@@ -19,10 +19,12 @@
     <sheet name="GA" sheetId="12" r:id="rId4"/>
     <sheet name="NC" sheetId="10" r:id="rId5"/>
     <sheet name="IL" sheetId="1" r:id="rId6"/>
-    <sheet name="OR" sheetId="9" r:id="rId7"/>
-    <sheet name="TX" sheetId="7" r:id="rId8"/>
-    <sheet name="UT" sheetId="2" r:id="rId9"/>
-    <sheet name="WA" sheetId="5" r:id="rId10"/>
+    <sheet name="MN" sheetId="13" r:id="rId7"/>
+    <sheet name="OR" sheetId="9" r:id="rId8"/>
+    <sheet name="TX" sheetId="7" r:id="rId9"/>
+    <sheet name="UT" sheetId="2" r:id="rId10"/>
+    <sheet name="WA" sheetId="5" r:id="rId11"/>
+    <sheet name="WI" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="824">
   <si>
     <t>sti</t>
   </si>
@@ -3451,6 +3453,85 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60086F-4E23-4552-812A-D6F349AB4AAA}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="G3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="G4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A7623CC5-2DD4-4C82-8E27-E943B9C67183}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E2328-4252-44D7-8F9F-0FEE326AAA47}">
   <dimension ref="A1:G40"/>
   <sheetViews>
@@ -3709,6 +3790,58 @@
     <hyperlink ref="G5" r:id="rId1" xr:uid="{89BAC0A9-74CB-4187-AD28-842BB73473FF}"/>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{F31759F6-49D6-4041-B8D6-8164FEB39454}"/>
     <hyperlink ref="G9" r:id="rId3" xr:uid="{7FC71B66-9A8A-4681-B6EC-1E7E9548D22D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E0E31F-B62D-4680-B1F4-A49EBE3A95E3}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6974CFCC-386B-41C5-B3C9-A434BC4CA775}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4758,7 +4891,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,7 +5895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
@@ -6926,6 +7059,62 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3763F8-F71B-49F5-BE31-3104EC77150F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{90A0AEB9-8A49-4607-B016-EB131DB3BD3F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3485B542-A7AE-49A8-9570-1F6A41EC410A}">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -7370,7 +7559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8813E460-3269-433D-A176-13509591D858}">
   <dimension ref="A1:G769"/>
   <sheetViews>
@@ -15861,83 +16050,4 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60086F-4E23-4552-812A-D6F349AB4AAA}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="G3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
-      <c r="G4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A7623CC5-2DD4-4C82-8E27-E943B9C67183}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update TX Lubbock fax
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4CC7CD-FC3A-49C7-B201-7C039C15235F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1948DBD-89B0-4D43-93CE-C8E5CE19D365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="827">
   <si>
     <t>sti</t>
   </si>
@@ -2794,12 +2794,15 @@
   <si>
     <t>MN_HEP_template.pdf</t>
   </si>
+  <si>
+    <t>806-775-3184</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2850,6 +2853,12 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2872,13 +2881,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3805,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E0E31F-B62D-4680-B1F4-A49EBE3A95E3}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7581,8 +7591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8813E460-3269-433D-A176-13509591D858}">
   <dimension ref="A1:G769"/>
   <sheetViews>
-    <sheetView topLeftCell="A734" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="E672" sqref="E672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14821,7 +14831,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A657" s="4" t="s">
         <v>733</v>
       </c>
@@ -14832,7 +14842,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A658" s="4" t="s">
         <v>734</v>
       </c>
@@ -14843,7 +14853,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A659" s="4" t="s">
         <v>97</v>
       </c>
@@ -14854,7 +14864,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A660" s="4" t="s">
         <v>318</v>
       </c>
@@ -14865,7 +14875,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A661" s="4" t="s">
         <v>533</v>
       </c>
@@ -14876,7 +14886,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A662" s="4" t="s">
         <v>735</v>
       </c>
@@ -14887,7 +14897,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A663" s="4" t="s">
         <v>736</v>
       </c>
@@ -14898,7 +14908,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A664" s="4" t="s">
         <v>737</v>
       </c>
@@ -14909,7 +14919,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="665" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A665" s="4" t="s">
         <v>319</v>
       </c>
@@ -14920,7 +14930,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A666" s="4" t="s">
         <v>738</v>
       </c>
@@ -14930,8 +14940,9 @@
       <c r="C666" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D666" s="6"/>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A667" s="4" t="s">
         <v>739</v>
       </c>
@@ -14939,10 +14950,10 @@
         <v>205</v>
       </c>
       <c r="C667" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A668" s="4" t="s">
         <v>740</v>
       </c>
@@ -14953,7 +14964,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A669" s="4" t="s">
         <v>741</v>
       </c>
@@ -14964,7 +14975,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A670" s="4" t="s">
         <v>742</v>
       </c>
@@ -14975,7 +14986,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="671" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A671" s="4" t="s">
         <v>744</v>
       </c>
@@ -14986,7 +14997,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A672" s="4" t="s">
         <v>107</v>
       </c>
@@ -16067,5 +16078,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add LA HEP template, update fields
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DDD5A9-AC89-46ED-8A82-4F05A82BD4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2926C6-2FB6-4E73-A46F-E1C2C6FF04AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4455" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4460" uniqueCount="832">
   <si>
     <t>sti</t>
   </si>
@@ -2803,6 +2803,15 @@
   </si>
   <si>
     <t>630-897-8128</t>
+  </si>
+  <si>
+    <t>GONO, CHLA, SYPH</t>
+  </si>
+  <si>
+    <t>HEP</t>
+  </si>
+  <si>
+    <t>LA_HEP_template.pdf</t>
   </si>
 </sst>
 </file>
@@ -17458,16 +17467,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A423D28C-3242-4F17-BAFA-5D15DE2DACDA}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
@@ -17499,12 +17508,29 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>829</v>
       </c>
       <c r="C2" t="s">
         <v>214</v>
       </c>
       <c r="E2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>830</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
+        <v>831</v>
+      </c>
+      <c r="E3" t="s">
         <v>291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disable CA, update WI
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B73E4C3-7E8A-459C-A290-0B967D9A3CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B702C67-CBFB-4856-9AFE-C8C8C5E1F854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="3" r:id="rId1"/>
-    <sheet name="CA" sheetId="6" r:id="rId2"/>
+    <sheet name="zCA" sheetId="6" r:id="rId2"/>
     <sheet name="FL" sheetId="11" r:id="rId3"/>
     <sheet name="GA" sheetId="12" r:id="rId4"/>
     <sheet name="IL" sheetId="1" r:id="rId5"/>
@@ -14668,7 +14668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABC6B03-4CD4-438B-B773-90767DEF6D87}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -17463,7 +17463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A423D28C-3242-4F17-BAFA-5D15DE2DACDA}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Appleton, WI target
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Usbtl-serv-pdc1\Users\nmirasol\My Documents\Misc\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA56D37-9E7B-43BC-9742-991375DB45D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA80A0-E80F-41C9-AAD2-1647E542ED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30060" yWindow="1470" windowWidth="17295" windowHeight="11835" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4470" uniqueCount="833">
   <si>
     <t>sti</t>
   </si>
@@ -2813,6 +2813,9 @@
   </si>
   <si>
     <t>WI</t>
+  </si>
+  <si>
+    <t>920-832-5853</t>
   </si>
 </sst>
 </file>
@@ -14676,13 +14679,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -14718,7 +14722,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>832</v>
       </c>
       <c r="E2" t="s">
         <v>291</v>

</xml_diff>